<commit_message>
Done clip Lập trình ReactJS - Bài 17 Sử dụng Ref: ref
</commit_message>
<xml_diff>
--- a/HocReactJS.xlsx
+++ b/HocReactJS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="01-03-2018" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>File App.js</t>
   </si>
@@ -24,12 +24,21 @@
   <si>
     <t>: clip Lập trình ReactJS - Bài 6 Tìm hiểu ReactJS phần 3</t>
   </si>
+  <si>
+    <t>File Course.js</t>
+  </si>
+  <si>
+    <t>Do this.props.name không hiểu là gì =&gt; dùng contructor</t>
+  </si>
+  <si>
+    <t>Ngày 2/2/2018</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,6 +51,13 @@
       <color theme="6"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,15 +80,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -116,7 +135,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -157,6 +176,98 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4695825" y="885825"/>
+          <a:ext cx="1133475" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>177998</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Capture.JPG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2190750"/>
+          <a:ext cx="4495800" cy="2844998"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Right Arrow 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4676775" y="3371850"/>
           <a:ext cx="1133475" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -236,7 +347,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,10 +379,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,7 +413,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -479,73 +588,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:16" ht="18.75">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="1"/>
       <c r="F2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K4" s="1" t="s">
+    <row r="4" spans="1:16">
+      <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="11" spans="1:16" ht="18.75">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="M11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="17" spans="11:16">
+      <c r="K17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="11:16">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="11:16">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="11:16">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="11:16">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="K4:P8"/>
     <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="K17:P21"/>
+    <mergeCell ref="M11:O11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Done clip 4.7: Các vấn đề nâng cao: ProductItem 01
</commit_message>
<xml_diff>
--- a/HocReactJS.xlsx
+++ b/HocReactJS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -37,8 +37,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,7 +135,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -347,7 +347,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,9 +379,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -413,6 +414,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -588,16 +590,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:16" ht="18.75">
+    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -609,7 +611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
@@ -619,7 +621,7 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -627,7 +629,7 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -635,7 +637,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -643,7 +645,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -651,7 +653,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="11" spans="1:16" ht="18.75">
+    <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -664,7 +666,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="17" spans="11:16">
+    <row r="17" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K17" s="2" t="s">
         <v>4</v>
       </c>
@@ -674,7 +676,7 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="11:16">
+    <row r="18" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -682,7 +684,7 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="11:16">
+    <row r="19" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -690,7 +692,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="11:16">
+    <row r="20" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -698,7 +700,7 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="11:16">
+    <row r="21" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>

</xml_diff>